<commit_message>
Add deny command, update actuator schema
</commit_message>
<xml_diff>
--- a/docs/targets.xlsx
+++ b/docs/targets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="122">
   <si>
     <t>Target Type</t>
   </si>
@@ -722,6 +722,43 @@
 }]
 </t>
   </si>
+  <si>
+    <t>{
+ "action": "deny",
+ "target": {
+  "ip-connection": {
+   "src-addr": {
+    "dns": {"value": "www.badco.com"}},
+   "src-port": {"protocol": "https"},
+   "dst-addr": {
+    "v4": {
+     "value": "192.168.1.1"}},
+   "layer4-protocol": "TCP"}},
+ "actuator": {
+  "network-firewall": {
+   "asset_id": "30"}},
+ "modifiers": {
+  "id": "pf17_8675309",
+  "context_ref": 91,
+  "datetime": "2016-11-25T08:10:31-04:00",
+  "duration": "PT2M30S"}}</t>
+  </si>
+  <si>
+    <t>[7, {
+ "15": [
+   {"4": ["www.badco.com"]},
+   {"2": 443},
+   {"1": ["192.168.1.1"]},
+   null,
+   null,
+   6]
+  },
+  {"14": [null, "30"]},
+  {"2": "PT2M30S",
+   "4": "2016-11-25T08:10:31-04:00",
+   "8": 91,
+   "9": "pf17_8675309"}]</t>
+  </si>
 </sst>
 </file>
 
@@ -1222,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
@@ -31451,8 +31488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -31460,7 +31497,7 @@
     <col min="1" max="1" width="16.85546875" style="20" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" style="18" customWidth="1"/>
     <col min="3" max="3" width="48.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="47" style="18" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
@@ -31625,8 +31662,12 @@
       <c r="B17" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="247.5">
       <c r="A18" s="22"/>

</xml_diff>

<commit_message>
Add example producer/consumer application
</commit_message>
<xml_diff>
--- a/docs/targets.xlsx
+++ b/docs/targets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835"/>
+    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
@@ -31486,10 +31486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D997"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -31787,2868 +31787,6 @@
     <row r="43" spans="1:1">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="2"/>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="2"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="2"/>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="2"/>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="2"/>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="2"/>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="2"/>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="2"/>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="2"/>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="2"/>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="2"/>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="2"/>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="2"/>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="2"/>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="2"/>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="2"/>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="2"/>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="2"/>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="2"/>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="2"/>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="2"/>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="2"/>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="2"/>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="2"/>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="2"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="2"/>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="2"/>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="2"/>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="2"/>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="2"/>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="2"/>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="2"/>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="2"/>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="2"/>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="2"/>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="2"/>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" s="2"/>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" s="2"/>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" s="2"/>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="2"/>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="2"/>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" s="2"/>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" s="2"/>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" s="2"/>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" s="2"/>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" s="2"/>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="2"/>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" s="2"/>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" s="2"/>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" s="2"/>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" s="2"/>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" s="2"/>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" s="2"/>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" s="2"/>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" s="2"/>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" s="2"/>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" s="2"/>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" s="2"/>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" s="2"/>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" s="2"/>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" s="2"/>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" s="2"/>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" s="2"/>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" s="2"/>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" s="2"/>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" s="2"/>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" s="2"/>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" s="2"/>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134" s="2"/>
-    </row>
-    <row r="135" spans="1:1">
-      <c r="A135" s="2"/>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136" s="2"/>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" s="2"/>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" s="2"/>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" s="2"/>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140" s="2"/>
-    </row>
-    <row r="141" spans="1:1">
-      <c r="A141" s="2"/>
-    </row>
-    <row r="142" spans="1:1">
-      <c r="A142" s="2"/>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143" s="2"/>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144" s="2"/>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145" s="2"/>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" s="2"/>
-    </row>
-    <row r="147" spans="1:1">
-      <c r="A147" s="2"/>
-    </row>
-    <row r="148" spans="1:1">
-      <c r="A148" s="2"/>
-    </row>
-    <row r="149" spans="1:1">
-      <c r="A149" s="2"/>
-    </row>
-    <row r="150" spans="1:1">
-      <c r="A150" s="2"/>
-    </row>
-    <row r="151" spans="1:1">
-      <c r="A151" s="2"/>
-    </row>
-    <row r="152" spans="1:1">
-      <c r="A152" s="2"/>
-    </row>
-    <row r="153" spans="1:1">
-      <c r="A153" s="2"/>
-    </row>
-    <row r="154" spans="1:1">
-      <c r="A154" s="2"/>
-    </row>
-    <row r="155" spans="1:1">
-      <c r="A155" s="2"/>
-    </row>
-    <row r="156" spans="1:1">
-      <c r="A156" s="2"/>
-    </row>
-    <row r="157" spans="1:1">
-      <c r="A157" s="2"/>
-    </row>
-    <row r="158" spans="1:1">
-      <c r="A158" s="2"/>
-    </row>
-    <row r="159" spans="1:1">
-      <c r="A159" s="2"/>
-    </row>
-    <row r="160" spans="1:1">
-      <c r="A160" s="2"/>
-    </row>
-    <row r="161" spans="1:1">
-      <c r="A161" s="2"/>
-    </row>
-    <row r="162" spans="1:1">
-      <c r="A162" s="2"/>
-    </row>
-    <row r="163" spans="1:1">
-      <c r="A163" s="2"/>
-    </row>
-    <row r="164" spans="1:1">
-      <c r="A164" s="2"/>
-    </row>
-    <row r="165" spans="1:1">
-      <c r="A165" s="2"/>
-    </row>
-    <row r="166" spans="1:1">
-      <c r="A166" s="2"/>
-    </row>
-    <row r="167" spans="1:1">
-      <c r="A167" s="2"/>
-    </row>
-    <row r="168" spans="1:1">
-      <c r="A168" s="2"/>
-    </row>
-    <row r="169" spans="1:1">
-      <c r="A169" s="2"/>
-    </row>
-    <row r="170" spans="1:1">
-      <c r="A170" s="2"/>
-    </row>
-    <row r="171" spans="1:1">
-      <c r="A171" s="2"/>
-    </row>
-    <row r="172" spans="1:1">
-      <c r="A172" s="2"/>
-    </row>
-    <row r="173" spans="1:1">
-      <c r="A173" s="2"/>
-    </row>
-    <row r="174" spans="1:1">
-      <c r="A174" s="2"/>
-    </row>
-    <row r="175" spans="1:1">
-      <c r="A175" s="2"/>
-    </row>
-    <row r="176" spans="1:1">
-      <c r="A176" s="2"/>
-    </row>
-    <row r="177" spans="1:1">
-      <c r="A177" s="2"/>
-    </row>
-    <row r="178" spans="1:1">
-      <c r="A178" s="2"/>
-    </row>
-    <row r="179" spans="1:1">
-      <c r="A179" s="2"/>
-    </row>
-    <row r="180" spans="1:1">
-      <c r="A180" s="2"/>
-    </row>
-    <row r="181" spans="1:1">
-      <c r="A181" s="2"/>
-    </row>
-    <row r="182" spans="1:1">
-      <c r="A182" s="2"/>
-    </row>
-    <row r="183" spans="1:1">
-      <c r="A183" s="2"/>
-    </row>
-    <row r="184" spans="1:1">
-      <c r="A184" s="2"/>
-    </row>
-    <row r="185" spans="1:1">
-      <c r="A185" s="2"/>
-    </row>
-    <row r="186" spans="1:1">
-      <c r="A186" s="2"/>
-    </row>
-    <row r="187" spans="1:1">
-      <c r="A187" s="2"/>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" s="2"/>
-    </row>
-    <row r="189" spans="1:1">
-      <c r="A189" s="2"/>
-    </row>
-    <row r="190" spans="1:1">
-      <c r="A190" s="2"/>
-    </row>
-    <row r="191" spans="1:1">
-      <c r="A191" s="2"/>
-    </row>
-    <row r="192" spans="1:1">
-      <c r="A192" s="2"/>
-    </row>
-    <row r="193" spans="1:1">
-      <c r="A193" s="2"/>
-    </row>
-    <row r="194" spans="1:1">
-      <c r="A194" s="2"/>
-    </row>
-    <row r="195" spans="1:1">
-      <c r="A195" s="2"/>
-    </row>
-    <row r="196" spans="1:1">
-      <c r="A196" s="2"/>
-    </row>
-    <row r="197" spans="1:1">
-      <c r="A197" s="2"/>
-    </row>
-    <row r="198" spans="1:1">
-      <c r="A198" s="2"/>
-    </row>
-    <row r="199" spans="1:1">
-      <c r="A199" s="2"/>
-    </row>
-    <row r="200" spans="1:1">
-      <c r="A200" s="2"/>
-    </row>
-    <row r="201" spans="1:1">
-      <c r="A201" s="2"/>
-    </row>
-    <row r="202" spans="1:1">
-      <c r="A202" s="2"/>
-    </row>
-    <row r="203" spans="1:1">
-      <c r="A203" s="2"/>
-    </row>
-    <row r="204" spans="1:1">
-      <c r="A204" s="2"/>
-    </row>
-    <row r="205" spans="1:1">
-      <c r="A205" s="2"/>
-    </row>
-    <row r="206" spans="1:1">
-      <c r="A206" s="2"/>
-    </row>
-    <row r="207" spans="1:1">
-      <c r="A207" s="2"/>
-    </row>
-    <row r="208" spans="1:1">
-      <c r="A208" s="2"/>
-    </row>
-    <row r="209" spans="1:1">
-      <c r="A209" s="2"/>
-    </row>
-    <row r="210" spans="1:1">
-      <c r="A210" s="2"/>
-    </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="2"/>
-    </row>
-    <row r="212" spans="1:1">
-      <c r="A212" s="2"/>
-    </row>
-    <row r="213" spans="1:1">
-      <c r="A213" s="2"/>
-    </row>
-    <row r="214" spans="1:1">
-      <c r="A214" s="2"/>
-    </row>
-    <row r="215" spans="1:1">
-      <c r="A215" s="2"/>
-    </row>
-    <row r="216" spans="1:1">
-      <c r="A216" s="2"/>
-    </row>
-    <row r="217" spans="1:1">
-      <c r="A217" s="2"/>
-    </row>
-    <row r="218" spans="1:1">
-      <c r="A218" s="2"/>
-    </row>
-    <row r="219" spans="1:1">
-      <c r="A219" s="2"/>
-    </row>
-    <row r="220" spans="1:1">
-      <c r="A220" s="2"/>
-    </row>
-    <row r="221" spans="1:1">
-      <c r="A221" s="2"/>
-    </row>
-    <row r="222" spans="1:1">
-      <c r="A222" s="2"/>
-    </row>
-    <row r="223" spans="1:1">
-      <c r="A223" s="2"/>
-    </row>
-    <row r="224" spans="1:1">
-      <c r="A224" s="2"/>
-    </row>
-    <row r="225" spans="1:1">
-      <c r="A225" s="2"/>
-    </row>
-    <row r="226" spans="1:1">
-      <c r="A226" s="2"/>
-    </row>
-    <row r="227" spans="1:1">
-      <c r="A227" s="2"/>
-    </row>
-    <row r="228" spans="1:1">
-      <c r="A228" s="2"/>
-    </row>
-    <row r="229" spans="1:1">
-      <c r="A229" s="2"/>
-    </row>
-    <row r="230" spans="1:1">
-      <c r="A230" s="2"/>
-    </row>
-    <row r="231" spans="1:1">
-      <c r="A231" s="2"/>
-    </row>
-    <row r="232" spans="1:1">
-      <c r="A232" s="2"/>
-    </row>
-    <row r="233" spans="1:1">
-      <c r="A233" s="2"/>
-    </row>
-    <row r="234" spans="1:1">
-      <c r="A234" s="2"/>
-    </row>
-    <row r="235" spans="1:1">
-      <c r="A235" s="2"/>
-    </row>
-    <row r="236" spans="1:1">
-      <c r="A236" s="2"/>
-    </row>
-    <row r="237" spans="1:1">
-      <c r="A237" s="2"/>
-    </row>
-    <row r="238" spans="1:1">
-      <c r="A238" s="2"/>
-    </row>
-    <row r="239" spans="1:1">
-      <c r="A239" s="2"/>
-    </row>
-    <row r="240" spans="1:1">
-      <c r="A240" s="2"/>
-    </row>
-    <row r="241" spans="1:1">
-      <c r="A241" s="2"/>
-    </row>
-    <row r="242" spans="1:1">
-      <c r="A242" s="2"/>
-    </row>
-    <row r="243" spans="1:1">
-      <c r="A243" s="2"/>
-    </row>
-    <row r="244" spans="1:1">
-      <c r="A244" s="2"/>
-    </row>
-    <row r="245" spans="1:1">
-      <c r="A245" s="2"/>
-    </row>
-    <row r="246" spans="1:1">
-      <c r="A246" s="2"/>
-    </row>
-    <row r="247" spans="1:1">
-      <c r="A247" s="2"/>
-    </row>
-    <row r="248" spans="1:1">
-      <c r="A248" s="2"/>
-    </row>
-    <row r="249" spans="1:1">
-      <c r="A249" s="2"/>
-    </row>
-    <row r="250" spans="1:1">
-      <c r="A250" s="2"/>
-    </row>
-    <row r="251" spans="1:1">
-      <c r="A251" s="2"/>
-    </row>
-    <row r="252" spans="1:1">
-      <c r="A252" s="2"/>
-    </row>
-    <row r="253" spans="1:1">
-      <c r="A253" s="2"/>
-    </row>
-    <row r="254" spans="1:1">
-      <c r="A254" s="2"/>
-    </row>
-    <row r="255" spans="1:1">
-      <c r="A255" s="2"/>
-    </row>
-    <row r="256" spans="1:1">
-      <c r="A256" s="2"/>
-    </row>
-    <row r="257" spans="1:1">
-      <c r="A257" s="2"/>
-    </row>
-    <row r="258" spans="1:1">
-      <c r="A258" s="2"/>
-    </row>
-    <row r="259" spans="1:1">
-      <c r="A259" s="2"/>
-    </row>
-    <row r="260" spans="1:1">
-      <c r="A260" s="2"/>
-    </row>
-    <row r="261" spans="1:1">
-      <c r="A261" s="2"/>
-    </row>
-    <row r="262" spans="1:1">
-      <c r="A262" s="2"/>
-    </row>
-    <row r="263" spans="1:1">
-      <c r="A263" s="2"/>
-    </row>
-    <row r="264" spans="1:1">
-      <c r="A264" s="2"/>
-    </row>
-    <row r="265" spans="1:1">
-      <c r="A265" s="2"/>
-    </row>
-    <row r="266" spans="1:1">
-      <c r="A266" s="2"/>
-    </row>
-    <row r="267" spans="1:1">
-      <c r="A267" s="2"/>
-    </row>
-    <row r="268" spans="1:1">
-      <c r="A268" s="2"/>
-    </row>
-    <row r="269" spans="1:1">
-      <c r="A269" s="2"/>
-    </row>
-    <row r="270" spans="1:1">
-      <c r="A270" s="2"/>
-    </row>
-    <row r="271" spans="1:1">
-      <c r="A271" s="2"/>
-    </row>
-    <row r="272" spans="1:1">
-      <c r="A272" s="2"/>
-    </row>
-    <row r="273" spans="1:1">
-      <c r="A273" s="2"/>
-    </row>
-    <row r="274" spans="1:1">
-      <c r="A274" s="2"/>
-    </row>
-    <row r="275" spans="1:1">
-      <c r="A275" s="2"/>
-    </row>
-    <row r="276" spans="1:1">
-      <c r="A276" s="2"/>
-    </row>
-    <row r="277" spans="1:1">
-      <c r="A277" s="2"/>
-    </row>
-    <row r="278" spans="1:1">
-      <c r="A278" s="2"/>
-    </row>
-    <row r="279" spans="1:1">
-      <c r="A279" s="2"/>
-    </row>
-    <row r="280" spans="1:1">
-      <c r="A280" s="2"/>
-    </row>
-    <row r="281" spans="1:1">
-      <c r="A281" s="2"/>
-    </row>
-    <row r="282" spans="1:1">
-      <c r="A282" s="2"/>
-    </row>
-    <row r="283" spans="1:1">
-      <c r="A283" s="2"/>
-    </row>
-    <row r="284" spans="1:1">
-      <c r="A284" s="2"/>
-    </row>
-    <row r="285" spans="1:1">
-      <c r="A285" s="2"/>
-    </row>
-    <row r="286" spans="1:1">
-      <c r="A286" s="2"/>
-    </row>
-    <row r="287" spans="1:1">
-      <c r="A287" s="2"/>
-    </row>
-    <row r="288" spans="1:1">
-      <c r="A288" s="2"/>
-    </row>
-    <row r="289" spans="1:1">
-      <c r="A289" s="2"/>
-    </row>
-    <row r="290" spans="1:1">
-      <c r="A290" s="2"/>
-    </row>
-    <row r="291" spans="1:1">
-      <c r="A291" s="2"/>
-    </row>
-    <row r="292" spans="1:1">
-      <c r="A292" s="2"/>
-    </row>
-    <row r="293" spans="1:1">
-      <c r="A293" s="2"/>
-    </row>
-    <row r="294" spans="1:1">
-      <c r="A294" s="2"/>
-    </row>
-    <row r="295" spans="1:1">
-      <c r="A295" s="2"/>
-    </row>
-    <row r="296" spans="1:1">
-      <c r="A296" s="2"/>
-    </row>
-    <row r="297" spans="1:1">
-      <c r="A297" s="2"/>
-    </row>
-    <row r="298" spans="1:1">
-      <c r="A298" s="2"/>
-    </row>
-    <row r="299" spans="1:1">
-      <c r="A299" s="2"/>
-    </row>
-    <row r="300" spans="1:1">
-      <c r="A300" s="2"/>
-    </row>
-    <row r="301" spans="1:1">
-      <c r="A301" s="2"/>
-    </row>
-    <row r="302" spans="1:1">
-      <c r="A302" s="2"/>
-    </row>
-    <row r="303" spans="1:1">
-      <c r="A303" s="2"/>
-    </row>
-    <row r="304" spans="1:1">
-      <c r="A304" s="2"/>
-    </row>
-    <row r="305" spans="1:1">
-      <c r="A305" s="2"/>
-    </row>
-    <row r="306" spans="1:1">
-      <c r="A306" s="2"/>
-    </row>
-    <row r="307" spans="1:1">
-      <c r="A307" s="2"/>
-    </row>
-    <row r="308" spans="1:1">
-      <c r="A308" s="2"/>
-    </row>
-    <row r="309" spans="1:1">
-      <c r="A309" s="2"/>
-    </row>
-    <row r="310" spans="1:1">
-      <c r="A310" s="2"/>
-    </row>
-    <row r="311" spans="1:1">
-      <c r="A311" s="2"/>
-    </row>
-    <row r="312" spans="1:1">
-      <c r="A312" s="2"/>
-    </row>
-    <row r="313" spans="1:1">
-      <c r="A313" s="2"/>
-    </row>
-    <row r="314" spans="1:1">
-      <c r="A314" s="2"/>
-    </row>
-    <row r="315" spans="1:1">
-      <c r="A315" s="2"/>
-    </row>
-    <row r="316" spans="1:1">
-      <c r="A316" s="2"/>
-    </row>
-    <row r="317" spans="1:1">
-      <c r="A317" s="2"/>
-    </row>
-    <row r="318" spans="1:1">
-      <c r="A318" s="2"/>
-    </row>
-    <row r="319" spans="1:1">
-      <c r="A319" s="2"/>
-    </row>
-    <row r="320" spans="1:1">
-      <c r="A320" s="2"/>
-    </row>
-    <row r="321" spans="1:1">
-      <c r="A321" s="2"/>
-    </row>
-    <row r="322" spans="1:1">
-      <c r="A322" s="2"/>
-    </row>
-    <row r="323" spans="1:1">
-      <c r="A323" s="2"/>
-    </row>
-    <row r="324" spans="1:1">
-      <c r="A324" s="2"/>
-    </row>
-    <row r="325" spans="1:1">
-      <c r="A325" s="2"/>
-    </row>
-    <row r="326" spans="1:1">
-      <c r="A326" s="2"/>
-    </row>
-    <row r="327" spans="1:1">
-      <c r="A327" s="2"/>
-    </row>
-    <row r="328" spans="1:1">
-      <c r="A328" s="2"/>
-    </row>
-    <row r="329" spans="1:1">
-      <c r="A329" s="2"/>
-    </row>
-    <row r="330" spans="1:1">
-      <c r="A330" s="2"/>
-    </row>
-    <row r="331" spans="1:1">
-      <c r="A331" s="2"/>
-    </row>
-    <row r="332" spans="1:1">
-      <c r="A332" s="2"/>
-    </row>
-    <row r="333" spans="1:1">
-      <c r="A333" s="2"/>
-    </row>
-    <row r="334" spans="1:1">
-      <c r="A334" s="2"/>
-    </row>
-    <row r="335" spans="1:1">
-      <c r="A335" s="2"/>
-    </row>
-    <row r="336" spans="1:1">
-      <c r="A336" s="2"/>
-    </row>
-    <row r="337" spans="1:1">
-      <c r="A337" s="2"/>
-    </row>
-    <row r="338" spans="1:1">
-      <c r="A338" s="2"/>
-    </row>
-    <row r="339" spans="1:1">
-      <c r="A339" s="2"/>
-    </row>
-    <row r="340" spans="1:1">
-      <c r="A340" s="2"/>
-    </row>
-    <row r="341" spans="1:1">
-      <c r="A341" s="2"/>
-    </row>
-    <row r="342" spans="1:1">
-      <c r="A342" s="2"/>
-    </row>
-    <row r="343" spans="1:1">
-      <c r="A343" s="2"/>
-    </row>
-    <row r="344" spans="1:1">
-      <c r="A344" s="2"/>
-    </row>
-    <row r="345" spans="1:1">
-      <c r="A345" s="2"/>
-    </row>
-    <row r="346" spans="1:1">
-      <c r="A346" s="2"/>
-    </row>
-    <row r="347" spans="1:1">
-      <c r="A347" s="2"/>
-    </row>
-    <row r="348" spans="1:1">
-      <c r="A348" s="2"/>
-    </row>
-    <row r="349" spans="1:1">
-      <c r="A349" s="2"/>
-    </row>
-    <row r="350" spans="1:1">
-      <c r="A350" s="2"/>
-    </row>
-    <row r="351" spans="1:1">
-      <c r="A351" s="2"/>
-    </row>
-    <row r="352" spans="1:1">
-      <c r="A352" s="2"/>
-    </row>
-    <row r="353" spans="1:1">
-      <c r="A353" s="2"/>
-    </row>
-    <row r="354" spans="1:1">
-      <c r="A354" s="2"/>
-    </row>
-    <row r="355" spans="1:1">
-      <c r="A355" s="2"/>
-    </row>
-    <row r="356" spans="1:1">
-      <c r="A356" s="2"/>
-    </row>
-    <row r="357" spans="1:1">
-      <c r="A357" s="2"/>
-    </row>
-    <row r="358" spans="1:1">
-      <c r="A358" s="2"/>
-    </row>
-    <row r="359" spans="1:1">
-      <c r="A359" s="2"/>
-    </row>
-    <row r="360" spans="1:1">
-      <c r="A360" s="2"/>
-    </row>
-    <row r="361" spans="1:1">
-      <c r="A361" s="2"/>
-    </row>
-    <row r="362" spans="1:1">
-      <c r="A362" s="2"/>
-    </row>
-    <row r="363" spans="1:1">
-      <c r="A363" s="2"/>
-    </row>
-    <row r="364" spans="1:1">
-      <c r="A364" s="2"/>
-    </row>
-    <row r="365" spans="1:1">
-      <c r="A365" s="2"/>
-    </row>
-    <row r="366" spans="1:1">
-      <c r="A366" s="2"/>
-    </row>
-    <row r="367" spans="1:1">
-      <c r="A367" s="2"/>
-    </row>
-    <row r="368" spans="1:1">
-      <c r="A368" s="2"/>
-    </row>
-    <row r="369" spans="1:1">
-      <c r="A369" s="2"/>
-    </row>
-    <row r="370" spans="1:1">
-      <c r="A370" s="2"/>
-    </row>
-    <row r="371" spans="1:1">
-      <c r="A371" s="2"/>
-    </row>
-    <row r="372" spans="1:1">
-      <c r="A372" s="2"/>
-    </row>
-    <row r="373" spans="1:1">
-      <c r="A373" s="2"/>
-    </row>
-    <row r="374" spans="1:1">
-      <c r="A374" s="2"/>
-    </row>
-    <row r="375" spans="1:1">
-      <c r="A375" s="2"/>
-    </row>
-    <row r="376" spans="1:1">
-      <c r="A376" s="2"/>
-    </row>
-    <row r="377" spans="1:1">
-      <c r="A377" s="2"/>
-    </row>
-    <row r="378" spans="1:1">
-      <c r="A378" s="2"/>
-    </row>
-    <row r="379" spans="1:1">
-      <c r="A379" s="2"/>
-    </row>
-    <row r="380" spans="1:1">
-      <c r="A380" s="2"/>
-    </row>
-    <row r="381" spans="1:1">
-      <c r="A381" s="2"/>
-    </row>
-    <row r="382" spans="1:1">
-      <c r="A382" s="2"/>
-    </row>
-    <row r="383" spans="1:1">
-      <c r="A383" s="2"/>
-    </row>
-    <row r="384" spans="1:1">
-      <c r="A384" s="2"/>
-    </row>
-    <row r="385" spans="1:1">
-      <c r="A385" s="2"/>
-    </row>
-    <row r="386" spans="1:1">
-      <c r="A386" s="2"/>
-    </row>
-    <row r="387" spans="1:1">
-      <c r="A387" s="2"/>
-    </row>
-    <row r="388" spans="1:1">
-      <c r="A388" s="2"/>
-    </row>
-    <row r="389" spans="1:1">
-      <c r="A389" s="2"/>
-    </row>
-    <row r="390" spans="1:1">
-      <c r="A390" s="2"/>
-    </row>
-    <row r="391" spans="1:1">
-      <c r="A391" s="2"/>
-    </row>
-    <row r="392" spans="1:1">
-      <c r="A392" s="2"/>
-    </row>
-    <row r="393" spans="1:1">
-      <c r="A393" s="2"/>
-    </row>
-    <row r="394" spans="1:1">
-      <c r="A394" s="2"/>
-    </row>
-    <row r="395" spans="1:1">
-      <c r="A395" s="2"/>
-    </row>
-    <row r="396" spans="1:1">
-      <c r="A396" s="2"/>
-    </row>
-    <row r="397" spans="1:1">
-      <c r="A397" s="2"/>
-    </row>
-    <row r="398" spans="1:1">
-      <c r="A398" s="2"/>
-    </row>
-    <row r="399" spans="1:1">
-      <c r="A399" s="2"/>
-    </row>
-    <row r="400" spans="1:1">
-      <c r="A400" s="2"/>
-    </row>
-    <row r="401" spans="1:1">
-      <c r="A401" s="2"/>
-    </row>
-    <row r="402" spans="1:1">
-      <c r="A402" s="2"/>
-    </row>
-    <row r="403" spans="1:1">
-      <c r="A403" s="2"/>
-    </row>
-    <row r="404" spans="1:1">
-      <c r="A404" s="2"/>
-    </row>
-    <row r="405" spans="1:1">
-      <c r="A405" s="2"/>
-    </row>
-    <row r="406" spans="1:1">
-      <c r="A406" s="2"/>
-    </row>
-    <row r="407" spans="1:1">
-      <c r="A407" s="2"/>
-    </row>
-    <row r="408" spans="1:1">
-      <c r="A408" s="2"/>
-    </row>
-    <row r="409" spans="1:1">
-      <c r="A409" s="2"/>
-    </row>
-    <row r="410" spans="1:1">
-      <c r="A410" s="2"/>
-    </row>
-    <row r="411" spans="1:1">
-      <c r="A411" s="2"/>
-    </row>
-    <row r="412" spans="1:1">
-      <c r="A412" s="2"/>
-    </row>
-    <row r="413" spans="1:1">
-      <c r="A413" s="2"/>
-    </row>
-    <row r="414" spans="1:1">
-      <c r="A414" s="2"/>
-    </row>
-    <row r="415" spans="1:1">
-      <c r="A415" s="2"/>
-    </row>
-    <row r="416" spans="1:1">
-      <c r="A416" s="2"/>
-    </row>
-    <row r="417" spans="1:1">
-      <c r="A417" s="2"/>
-    </row>
-    <row r="418" spans="1:1">
-      <c r="A418" s="2"/>
-    </row>
-    <row r="419" spans="1:1">
-      <c r="A419" s="2"/>
-    </row>
-    <row r="420" spans="1:1">
-      <c r="A420" s="2"/>
-    </row>
-    <row r="421" spans="1:1">
-      <c r="A421" s="2"/>
-    </row>
-    <row r="422" spans="1:1">
-      <c r="A422" s="2"/>
-    </row>
-    <row r="423" spans="1:1">
-      <c r="A423" s="2"/>
-    </row>
-    <row r="424" spans="1:1">
-      <c r="A424" s="2"/>
-    </row>
-    <row r="425" spans="1:1">
-      <c r="A425" s="2"/>
-    </row>
-    <row r="426" spans="1:1">
-      <c r="A426" s="2"/>
-    </row>
-    <row r="427" spans="1:1">
-      <c r="A427" s="2"/>
-    </row>
-    <row r="428" spans="1:1">
-      <c r="A428" s="2"/>
-    </row>
-    <row r="429" spans="1:1">
-      <c r="A429" s="2"/>
-    </row>
-    <row r="430" spans="1:1">
-      <c r="A430" s="2"/>
-    </row>
-    <row r="431" spans="1:1">
-      <c r="A431" s="2"/>
-    </row>
-    <row r="432" spans="1:1">
-      <c r="A432" s="2"/>
-    </row>
-    <row r="433" spans="1:1">
-      <c r="A433" s="2"/>
-    </row>
-    <row r="434" spans="1:1">
-      <c r="A434" s="2"/>
-    </row>
-    <row r="435" spans="1:1">
-      <c r="A435" s="2"/>
-    </row>
-    <row r="436" spans="1:1">
-      <c r="A436" s="2"/>
-    </row>
-    <row r="437" spans="1:1">
-      <c r="A437" s="2"/>
-    </row>
-    <row r="438" spans="1:1">
-      <c r="A438" s="2"/>
-    </row>
-    <row r="439" spans="1:1">
-      <c r="A439" s="2"/>
-    </row>
-    <row r="440" spans="1:1">
-      <c r="A440" s="2"/>
-    </row>
-    <row r="441" spans="1:1">
-      <c r="A441" s="2"/>
-    </row>
-    <row r="442" spans="1:1">
-      <c r="A442" s="2"/>
-    </row>
-    <row r="443" spans="1:1">
-      <c r="A443" s="2"/>
-    </row>
-    <row r="444" spans="1:1">
-      <c r="A444" s="2"/>
-    </row>
-    <row r="445" spans="1:1">
-      <c r="A445" s="2"/>
-    </row>
-    <row r="446" spans="1:1">
-      <c r="A446" s="2"/>
-    </row>
-    <row r="447" spans="1:1">
-      <c r="A447" s="2"/>
-    </row>
-    <row r="448" spans="1:1">
-      <c r="A448" s="2"/>
-    </row>
-    <row r="449" spans="1:1">
-      <c r="A449" s="2"/>
-    </row>
-    <row r="450" spans="1:1">
-      <c r="A450" s="2"/>
-    </row>
-    <row r="451" spans="1:1">
-      <c r="A451" s="2"/>
-    </row>
-    <row r="452" spans="1:1">
-      <c r="A452" s="2"/>
-    </row>
-    <row r="453" spans="1:1">
-      <c r="A453" s="2"/>
-    </row>
-    <row r="454" spans="1:1">
-      <c r="A454" s="2"/>
-    </row>
-    <row r="455" spans="1:1">
-      <c r="A455" s="2"/>
-    </row>
-    <row r="456" spans="1:1">
-      <c r="A456" s="2"/>
-    </row>
-    <row r="457" spans="1:1">
-      <c r="A457" s="2"/>
-    </row>
-    <row r="458" spans="1:1">
-      <c r="A458" s="2"/>
-    </row>
-    <row r="459" spans="1:1">
-      <c r="A459" s="2"/>
-    </row>
-    <row r="460" spans="1:1">
-      <c r="A460" s="2"/>
-    </row>
-    <row r="461" spans="1:1">
-      <c r="A461" s="2"/>
-    </row>
-    <row r="462" spans="1:1">
-      <c r="A462" s="2"/>
-    </row>
-    <row r="463" spans="1:1">
-      <c r="A463" s="2"/>
-    </row>
-    <row r="464" spans="1:1">
-      <c r="A464" s="2"/>
-    </row>
-    <row r="465" spans="1:1">
-      <c r="A465" s="2"/>
-    </row>
-    <row r="466" spans="1:1">
-      <c r="A466" s="2"/>
-    </row>
-    <row r="467" spans="1:1">
-      <c r="A467" s="2"/>
-    </row>
-    <row r="468" spans="1:1">
-      <c r="A468" s="2"/>
-    </row>
-    <row r="469" spans="1:1">
-      <c r="A469" s="2"/>
-    </row>
-    <row r="470" spans="1:1">
-      <c r="A470" s="2"/>
-    </row>
-    <row r="471" spans="1:1">
-      <c r="A471" s="2"/>
-    </row>
-    <row r="472" spans="1:1">
-      <c r="A472" s="2"/>
-    </row>
-    <row r="473" spans="1:1">
-      <c r="A473" s="2"/>
-    </row>
-    <row r="474" spans="1:1">
-      <c r="A474" s="2"/>
-    </row>
-    <row r="475" spans="1:1">
-      <c r="A475" s="2"/>
-    </row>
-    <row r="476" spans="1:1">
-      <c r="A476" s="2"/>
-    </row>
-    <row r="477" spans="1:1">
-      <c r="A477" s="2"/>
-    </row>
-    <row r="478" spans="1:1">
-      <c r="A478" s="2"/>
-    </row>
-    <row r="479" spans="1:1">
-      <c r="A479" s="2"/>
-    </row>
-    <row r="480" spans="1:1">
-      <c r="A480" s="2"/>
-    </row>
-    <row r="481" spans="1:1">
-      <c r="A481" s="2"/>
-    </row>
-    <row r="482" spans="1:1">
-      <c r="A482" s="2"/>
-    </row>
-    <row r="483" spans="1:1">
-      <c r="A483" s="2"/>
-    </row>
-    <row r="484" spans="1:1">
-      <c r="A484" s="2"/>
-    </row>
-    <row r="485" spans="1:1">
-      <c r="A485" s="2"/>
-    </row>
-    <row r="486" spans="1:1">
-      <c r="A486" s="2"/>
-    </row>
-    <row r="487" spans="1:1">
-      <c r="A487" s="2"/>
-    </row>
-    <row r="488" spans="1:1">
-      <c r="A488" s="2"/>
-    </row>
-    <row r="489" spans="1:1">
-      <c r="A489" s="2"/>
-    </row>
-    <row r="490" spans="1:1">
-      <c r="A490" s="2"/>
-    </row>
-    <row r="491" spans="1:1">
-      <c r="A491" s="2"/>
-    </row>
-    <row r="492" spans="1:1">
-      <c r="A492" s="2"/>
-    </row>
-    <row r="493" spans="1:1">
-      <c r="A493" s="2"/>
-    </row>
-    <row r="494" spans="1:1">
-      <c r="A494" s="2"/>
-    </row>
-    <row r="495" spans="1:1">
-      <c r="A495" s="2"/>
-    </row>
-    <row r="496" spans="1:1">
-      <c r="A496" s="2"/>
-    </row>
-    <row r="497" spans="1:1">
-      <c r="A497" s="2"/>
-    </row>
-    <row r="498" spans="1:1">
-      <c r="A498" s="2"/>
-    </row>
-    <row r="499" spans="1:1">
-      <c r="A499" s="2"/>
-    </row>
-    <row r="500" spans="1:1">
-      <c r="A500" s="2"/>
-    </row>
-    <row r="501" spans="1:1">
-      <c r="A501" s="2"/>
-    </row>
-    <row r="502" spans="1:1">
-      <c r="A502" s="2"/>
-    </row>
-    <row r="503" spans="1:1">
-      <c r="A503" s="2"/>
-    </row>
-    <row r="504" spans="1:1">
-      <c r="A504" s="2"/>
-    </row>
-    <row r="505" spans="1:1">
-      <c r="A505" s="2"/>
-    </row>
-    <row r="506" spans="1:1">
-      <c r="A506" s="2"/>
-    </row>
-    <row r="507" spans="1:1">
-      <c r="A507" s="2"/>
-    </row>
-    <row r="508" spans="1:1">
-      <c r="A508" s="2"/>
-    </row>
-    <row r="509" spans="1:1">
-      <c r="A509" s="2"/>
-    </row>
-    <row r="510" spans="1:1">
-      <c r="A510" s="2"/>
-    </row>
-    <row r="511" spans="1:1">
-      <c r="A511" s="2"/>
-    </row>
-    <row r="512" spans="1:1">
-      <c r="A512" s="2"/>
-    </row>
-    <row r="513" spans="1:1">
-      <c r="A513" s="2"/>
-    </row>
-    <row r="514" spans="1:1">
-      <c r="A514" s="2"/>
-    </row>
-    <row r="515" spans="1:1">
-      <c r="A515" s="2"/>
-    </row>
-    <row r="516" spans="1:1">
-      <c r="A516" s="2"/>
-    </row>
-    <row r="517" spans="1:1">
-      <c r="A517" s="2"/>
-    </row>
-    <row r="518" spans="1:1">
-      <c r="A518" s="2"/>
-    </row>
-    <row r="519" spans="1:1">
-      <c r="A519" s="2"/>
-    </row>
-    <row r="520" spans="1:1">
-      <c r="A520" s="2"/>
-    </row>
-    <row r="521" spans="1:1">
-      <c r="A521" s="2"/>
-    </row>
-    <row r="522" spans="1:1">
-      <c r="A522" s="2"/>
-    </row>
-    <row r="523" spans="1:1">
-      <c r="A523" s="2"/>
-    </row>
-    <row r="524" spans="1:1">
-      <c r="A524" s="2"/>
-    </row>
-    <row r="525" spans="1:1">
-      <c r="A525" s="2"/>
-    </row>
-    <row r="526" spans="1:1">
-      <c r="A526" s="2"/>
-    </row>
-    <row r="527" spans="1:1">
-      <c r="A527" s="2"/>
-    </row>
-    <row r="528" spans="1:1">
-      <c r="A528" s="2"/>
-    </row>
-    <row r="529" spans="1:1">
-      <c r="A529" s="2"/>
-    </row>
-    <row r="530" spans="1:1">
-      <c r="A530" s="2"/>
-    </row>
-    <row r="531" spans="1:1">
-      <c r="A531" s="2"/>
-    </row>
-    <row r="532" spans="1:1">
-      <c r="A532" s="2"/>
-    </row>
-    <row r="533" spans="1:1">
-      <c r="A533" s="2"/>
-    </row>
-    <row r="534" spans="1:1">
-      <c r="A534" s="2"/>
-    </row>
-    <row r="535" spans="1:1">
-      <c r="A535" s="2"/>
-    </row>
-    <row r="536" spans="1:1">
-      <c r="A536" s="2"/>
-    </row>
-    <row r="537" spans="1:1">
-      <c r="A537" s="2"/>
-    </row>
-    <row r="538" spans="1:1">
-      <c r="A538" s="2"/>
-    </row>
-    <row r="539" spans="1:1">
-      <c r="A539" s="2"/>
-    </row>
-    <row r="540" spans="1:1">
-      <c r="A540" s="2"/>
-    </row>
-    <row r="541" spans="1:1">
-      <c r="A541" s="2"/>
-    </row>
-    <row r="542" spans="1:1">
-      <c r="A542" s="2"/>
-    </row>
-    <row r="543" spans="1:1">
-      <c r="A543" s="2"/>
-    </row>
-    <row r="544" spans="1:1">
-      <c r="A544" s="2"/>
-    </row>
-    <row r="545" spans="1:1">
-      <c r="A545" s="2"/>
-    </row>
-    <row r="546" spans="1:1">
-      <c r="A546" s="2"/>
-    </row>
-    <row r="547" spans="1:1">
-      <c r="A547" s="2"/>
-    </row>
-    <row r="548" spans="1:1">
-      <c r="A548" s="2"/>
-    </row>
-    <row r="549" spans="1:1">
-      <c r="A549" s="2"/>
-    </row>
-    <row r="550" spans="1:1">
-      <c r="A550" s="2"/>
-    </row>
-    <row r="551" spans="1:1">
-      <c r="A551" s="2"/>
-    </row>
-    <row r="552" spans="1:1">
-      <c r="A552" s="2"/>
-    </row>
-    <row r="553" spans="1:1">
-      <c r="A553" s="2"/>
-    </row>
-    <row r="554" spans="1:1">
-      <c r="A554" s="2"/>
-    </row>
-    <row r="555" spans="1:1">
-      <c r="A555" s="2"/>
-    </row>
-    <row r="556" spans="1:1">
-      <c r="A556" s="2"/>
-    </row>
-    <row r="557" spans="1:1">
-      <c r="A557" s="2"/>
-    </row>
-    <row r="558" spans="1:1">
-      <c r="A558" s="2"/>
-    </row>
-    <row r="559" spans="1:1">
-      <c r="A559" s="2"/>
-    </row>
-    <row r="560" spans="1:1">
-      <c r="A560" s="2"/>
-    </row>
-    <row r="561" spans="1:1">
-      <c r="A561" s="2"/>
-    </row>
-    <row r="562" spans="1:1">
-      <c r="A562" s="2"/>
-    </row>
-    <row r="563" spans="1:1">
-      <c r="A563" s="2"/>
-    </row>
-    <row r="564" spans="1:1">
-      <c r="A564" s="2"/>
-    </row>
-    <row r="565" spans="1:1">
-      <c r="A565" s="2"/>
-    </row>
-    <row r="566" spans="1:1">
-      <c r="A566" s="2"/>
-    </row>
-    <row r="567" spans="1:1">
-      <c r="A567" s="2"/>
-    </row>
-    <row r="568" spans="1:1">
-      <c r="A568" s="2"/>
-    </row>
-    <row r="569" spans="1:1">
-      <c r="A569" s="2"/>
-    </row>
-    <row r="570" spans="1:1">
-      <c r="A570" s="2"/>
-    </row>
-    <row r="571" spans="1:1">
-      <c r="A571" s="2"/>
-    </row>
-    <row r="572" spans="1:1">
-      <c r="A572" s="2"/>
-    </row>
-    <row r="573" spans="1:1">
-      <c r="A573" s="2"/>
-    </row>
-    <row r="574" spans="1:1">
-      <c r="A574" s="2"/>
-    </row>
-    <row r="575" spans="1:1">
-      <c r="A575" s="2"/>
-    </row>
-    <row r="576" spans="1:1">
-      <c r="A576" s="2"/>
-    </row>
-    <row r="577" spans="1:1">
-      <c r="A577" s="2"/>
-    </row>
-    <row r="578" spans="1:1">
-      <c r="A578" s="2"/>
-    </row>
-    <row r="579" spans="1:1">
-      <c r="A579" s="2"/>
-    </row>
-    <row r="580" spans="1:1">
-      <c r="A580" s="2"/>
-    </row>
-    <row r="581" spans="1:1">
-      <c r="A581" s="2"/>
-    </row>
-    <row r="582" spans="1:1">
-      <c r="A582" s="2"/>
-    </row>
-    <row r="583" spans="1:1">
-      <c r="A583" s="2"/>
-    </row>
-    <row r="584" spans="1:1">
-      <c r="A584" s="2"/>
-    </row>
-    <row r="585" spans="1:1">
-      <c r="A585" s="2"/>
-    </row>
-    <row r="586" spans="1:1">
-      <c r="A586" s="2"/>
-    </row>
-    <row r="587" spans="1:1">
-      <c r="A587" s="2"/>
-    </row>
-    <row r="588" spans="1:1">
-      <c r="A588" s="2"/>
-    </row>
-    <row r="589" spans="1:1">
-      <c r="A589" s="2"/>
-    </row>
-    <row r="590" spans="1:1">
-      <c r="A590" s="2"/>
-    </row>
-    <row r="591" spans="1:1">
-      <c r="A591" s="2"/>
-    </row>
-    <row r="592" spans="1:1">
-      <c r="A592" s="2"/>
-    </row>
-    <row r="593" spans="1:1">
-      <c r="A593" s="2"/>
-    </row>
-    <row r="594" spans="1:1">
-      <c r="A594" s="2"/>
-    </row>
-    <row r="595" spans="1:1">
-      <c r="A595" s="2"/>
-    </row>
-    <row r="596" spans="1:1">
-      <c r="A596" s="2"/>
-    </row>
-    <row r="597" spans="1:1">
-      <c r="A597" s="2"/>
-    </row>
-    <row r="598" spans="1:1">
-      <c r="A598" s="2"/>
-    </row>
-    <row r="599" spans="1:1">
-      <c r="A599" s="2"/>
-    </row>
-    <row r="600" spans="1:1">
-      <c r="A600" s="2"/>
-    </row>
-    <row r="601" spans="1:1">
-      <c r="A601" s="2"/>
-    </row>
-    <row r="602" spans="1:1">
-      <c r="A602" s="2"/>
-    </row>
-    <row r="603" spans="1:1">
-      <c r="A603" s="2"/>
-    </row>
-    <row r="604" spans="1:1">
-      <c r="A604" s="2"/>
-    </row>
-    <row r="605" spans="1:1">
-      <c r="A605" s="2"/>
-    </row>
-    <row r="606" spans="1:1">
-      <c r="A606" s="2"/>
-    </row>
-    <row r="607" spans="1:1">
-      <c r="A607" s="2"/>
-    </row>
-    <row r="608" spans="1:1">
-      <c r="A608" s="2"/>
-    </row>
-    <row r="609" spans="1:1">
-      <c r="A609" s="2"/>
-    </row>
-    <row r="610" spans="1:1">
-      <c r="A610" s="2"/>
-    </row>
-    <row r="611" spans="1:1">
-      <c r="A611" s="2"/>
-    </row>
-    <row r="612" spans="1:1">
-      <c r="A612" s="2"/>
-    </row>
-    <row r="613" spans="1:1">
-      <c r="A613" s="2"/>
-    </row>
-    <row r="614" spans="1:1">
-      <c r="A614" s="2"/>
-    </row>
-    <row r="615" spans="1:1">
-      <c r="A615" s="2"/>
-    </row>
-    <row r="616" spans="1:1">
-      <c r="A616" s="2"/>
-    </row>
-    <row r="617" spans="1:1">
-      <c r="A617" s="2"/>
-    </row>
-    <row r="618" spans="1:1">
-      <c r="A618" s="2"/>
-    </row>
-    <row r="619" spans="1:1">
-      <c r="A619" s="2"/>
-    </row>
-    <row r="620" spans="1:1">
-      <c r="A620" s="2"/>
-    </row>
-    <row r="621" spans="1:1">
-      <c r="A621" s="2"/>
-    </row>
-    <row r="622" spans="1:1">
-      <c r="A622" s="2"/>
-    </row>
-    <row r="623" spans="1:1">
-      <c r="A623" s="2"/>
-    </row>
-    <row r="624" spans="1:1">
-      <c r="A624" s="2"/>
-    </row>
-    <row r="625" spans="1:1">
-      <c r="A625" s="2"/>
-    </row>
-    <row r="626" spans="1:1">
-      <c r="A626" s="2"/>
-    </row>
-    <row r="627" spans="1:1">
-      <c r="A627" s="2"/>
-    </row>
-    <row r="628" spans="1:1">
-      <c r="A628" s="2"/>
-    </row>
-    <row r="629" spans="1:1">
-      <c r="A629" s="2"/>
-    </row>
-    <row r="630" spans="1:1">
-      <c r="A630" s="2"/>
-    </row>
-    <row r="631" spans="1:1">
-      <c r="A631" s="2"/>
-    </row>
-    <row r="632" spans="1:1">
-      <c r="A632" s="2"/>
-    </row>
-    <row r="633" spans="1:1">
-      <c r="A633" s="2"/>
-    </row>
-    <row r="634" spans="1:1">
-      <c r="A634" s="2"/>
-    </row>
-    <row r="635" spans="1:1">
-      <c r="A635" s="2"/>
-    </row>
-    <row r="636" spans="1:1">
-      <c r="A636" s="2"/>
-    </row>
-    <row r="637" spans="1:1">
-      <c r="A637" s="2"/>
-    </row>
-    <row r="638" spans="1:1">
-      <c r="A638" s="2"/>
-    </row>
-    <row r="639" spans="1:1">
-      <c r="A639" s="2"/>
-    </row>
-    <row r="640" spans="1:1">
-      <c r="A640" s="2"/>
-    </row>
-    <row r="641" spans="1:1">
-      <c r="A641" s="2"/>
-    </row>
-    <row r="642" spans="1:1">
-      <c r="A642" s="2"/>
-    </row>
-    <row r="643" spans="1:1">
-      <c r="A643" s="2"/>
-    </row>
-    <row r="644" spans="1:1">
-      <c r="A644" s="2"/>
-    </row>
-    <row r="645" spans="1:1">
-      <c r="A645" s="2"/>
-    </row>
-    <row r="646" spans="1:1">
-      <c r="A646" s="2"/>
-    </row>
-    <row r="647" spans="1:1">
-      <c r="A647" s="2"/>
-    </row>
-    <row r="648" spans="1:1">
-      <c r="A648" s="2"/>
-    </row>
-    <row r="649" spans="1:1">
-      <c r="A649" s="2"/>
-    </row>
-    <row r="650" spans="1:1">
-      <c r="A650" s="2"/>
-    </row>
-    <row r="651" spans="1:1">
-      <c r="A651" s="2"/>
-    </row>
-    <row r="652" spans="1:1">
-      <c r="A652" s="2"/>
-    </row>
-    <row r="653" spans="1:1">
-      <c r="A653" s="2"/>
-    </row>
-    <row r="654" spans="1:1">
-      <c r="A654" s="2"/>
-    </row>
-    <row r="655" spans="1:1">
-      <c r="A655" s="2"/>
-    </row>
-    <row r="656" spans="1:1">
-      <c r="A656" s="2"/>
-    </row>
-    <row r="657" spans="1:1">
-      <c r="A657" s="2"/>
-    </row>
-    <row r="658" spans="1:1">
-      <c r="A658" s="2"/>
-    </row>
-    <row r="659" spans="1:1">
-      <c r="A659" s="2"/>
-    </row>
-    <row r="660" spans="1:1">
-      <c r="A660" s="2"/>
-    </row>
-    <row r="661" spans="1:1">
-      <c r="A661" s="2"/>
-    </row>
-    <row r="662" spans="1:1">
-      <c r="A662" s="2"/>
-    </row>
-    <row r="663" spans="1:1">
-      <c r="A663" s="2"/>
-    </row>
-    <row r="664" spans="1:1">
-      <c r="A664" s="2"/>
-    </row>
-    <row r="665" spans="1:1">
-      <c r="A665" s="2"/>
-    </row>
-    <row r="666" spans="1:1">
-      <c r="A666" s="2"/>
-    </row>
-    <row r="667" spans="1:1">
-      <c r="A667" s="2"/>
-    </row>
-    <row r="668" spans="1:1">
-      <c r="A668" s="2"/>
-    </row>
-    <row r="669" spans="1:1">
-      <c r="A669" s="2"/>
-    </row>
-    <row r="670" spans="1:1">
-      <c r="A670" s="2"/>
-    </row>
-    <row r="671" spans="1:1">
-      <c r="A671" s="2"/>
-    </row>
-    <row r="672" spans="1:1">
-      <c r="A672" s="2"/>
-    </row>
-    <row r="673" spans="1:1">
-      <c r="A673" s="2"/>
-    </row>
-    <row r="674" spans="1:1">
-      <c r="A674" s="2"/>
-    </row>
-    <row r="675" spans="1:1">
-      <c r="A675" s="2"/>
-    </row>
-    <row r="676" spans="1:1">
-      <c r="A676" s="2"/>
-    </row>
-    <row r="677" spans="1:1">
-      <c r="A677" s="2"/>
-    </row>
-    <row r="678" spans="1:1">
-      <c r="A678" s="2"/>
-    </row>
-    <row r="679" spans="1:1">
-      <c r="A679" s="2"/>
-    </row>
-    <row r="680" spans="1:1">
-      <c r="A680" s="2"/>
-    </row>
-    <row r="681" spans="1:1">
-      <c r="A681" s="2"/>
-    </row>
-    <row r="682" spans="1:1">
-      <c r="A682" s="2"/>
-    </row>
-    <row r="683" spans="1:1">
-      <c r="A683" s="2"/>
-    </row>
-    <row r="684" spans="1:1">
-      <c r="A684" s="2"/>
-    </row>
-    <row r="685" spans="1:1">
-      <c r="A685" s="2"/>
-    </row>
-    <row r="686" spans="1:1">
-      <c r="A686" s="2"/>
-    </row>
-    <row r="687" spans="1:1">
-      <c r="A687" s="2"/>
-    </row>
-    <row r="688" spans="1:1">
-      <c r="A688" s="2"/>
-    </row>
-    <row r="689" spans="1:1">
-      <c r="A689" s="2"/>
-    </row>
-    <row r="690" spans="1:1">
-      <c r="A690" s="2"/>
-    </row>
-    <row r="691" spans="1:1">
-      <c r="A691" s="2"/>
-    </row>
-    <row r="692" spans="1:1">
-      <c r="A692" s="2"/>
-    </row>
-    <row r="693" spans="1:1">
-      <c r="A693" s="2"/>
-    </row>
-    <row r="694" spans="1:1">
-      <c r="A694" s="2"/>
-    </row>
-    <row r="695" spans="1:1">
-      <c r="A695" s="2"/>
-    </row>
-    <row r="696" spans="1:1">
-      <c r="A696" s="2"/>
-    </row>
-    <row r="697" spans="1:1">
-      <c r="A697" s="2"/>
-    </row>
-    <row r="698" spans="1:1">
-      <c r="A698" s="2"/>
-    </row>
-    <row r="699" spans="1:1">
-      <c r="A699" s="2"/>
-    </row>
-    <row r="700" spans="1:1">
-      <c r="A700" s="2"/>
-    </row>
-    <row r="701" spans="1:1">
-      <c r="A701" s="2"/>
-    </row>
-    <row r="702" spans="1:1">
-      <c r="A702" s="2"/>
-    </row>
-    <row r="703" spans="1:1">
-      <c r="A703" s="2"/>
-    </row>
-    <row r="704" spans="1:1">
-      <c r="A704" s="2"/>
-    </row>
-    <row r="705" spans="1:1">
-      <c r="A705" s="2"/>
-    </row>
-    <row r="706" spans="1:1">
-      <c r="A706" s="2"/>
-    </row>
-    <row r="707" spans="1:1">
-      <c r="A707" s="2"/>
-    </row>
-    <row r="708" spans="1:1">
-      <c r="A708" s="2"/>
-    </row>
-    <row r="709" spans="1:1">
-      <c r="A709" s="2"/>
-    </row>
-    <row r="710" spans="1:1">
-      <c r="A710" s="2"/>
-    </row>
-    <row r="711" spans="1:1">
-      <c r="A711" s="2"/>
-    </row>
-    <row r="712" spans="1:1">
-      <c r="A712" s="2"/>
-    </row>
-    <row r="713" spans="1:1">
-      <c r="A713" s="2"/>
-    </row>
-    <row r="714" spans="1:1">
-      <c r="A714" s="2"/>
-    </row>
-    <row r="715" spans="1:1">
-      <c r="A715" s="2"/>
-    </row>
-    <row r="716" spans="1:1">
-      <c r="A716" s="2"/>
-    </row>
-    <row r="717" spans="1:1">
-      <c r="A717" s="2"/>
-    </row>
-    <row r="718" spans="1:1">
-      <c r="A718" s="2"/>
-    </row>
-    <row r="719" spans="1:1">
-      <c r="A719" s="2"/>
-    </row>
-    <row r="720" spans="1:1">
-      <c r="A720" s="2"/>
-    </row>
-    <row r="721" spans="1:1">
-      <c r="A721" s="2"/>
-    </row>
-    <row r="722" spans="1:1">
-      <c r="A722" s="2"/>
-    </row>
-    <row r="723" spans="1:1">
-      <c r="A723" s="2"/>
-    </row>
-    <row r="724" spans="1:1">
-      <c r="A724" s="2"/>
-    </row>
-    <row r="725" spans="1:1">
-      <c r="A725" s="2"/>
-    </row>
-    <row r="726" spans="1:1">
-      <c r="A726" s="2"/>
-    </row>
-    <row r="727" spans="1:1">
-      <c r="A727" s="2"/>
-    </row>
-    <row r="728" spans="1:1">
-      <c r="A728" s="2"/>
-    </row>
-    <row r="729" spans="1:1">
-      <c r="A729" s="2"/>
-    </row>
-    <row r="730" spans="1:1">
-      <c r="A730" s="2"/>
-    </row>
-    <row r="731" spans="1:1">
-      <c r="A731" s="2"/>
-    </row>
-    <row r="732" spans="1:1">
-      <c r="A732" s="2"/>
-    </row>
-    <row r="733" spans="1:1">
-      <c r="A733" s="2"/>
-    </row>
-    <row r="734" spans="1:1">
-      <c r="A734" s="2"/>
-    </row>
-    <row r="735" spans="1:1">
-      <c r="A735" s="2"/>
-    </row>
-    <row r="736" spans="1:1">
-      <c r="A736" s="2"/>
-    </row>
-    <row r="737" spans="1:1">
-      <c r="A737" s="2"/>
-    </row>
-    <row r="738" spans="1:1">
-      <c r="A738" s="2"/>
-    </row>
-    <row r="739" spans="1:1">
-      <c r="A739" s="2"/>
-    </row>
-    <row r="740" spans="1:1">
-      <c r="A740" s="2"/>
-    </row>
-    <row r="741" spans="1:1">
-      <c r="A741" s="2"/>
-    </row>
-    <row r="742" spans="1:1">
-      <c r="A742" s="2"/>
-    </row>
-    <row r="743" spans="1:1">
-      <c r="A743" s="2"/>
-    </row>
-    <row r="744" spans="1:1">
-      <c r="A744" s="2"/>
-    </row>
-    <row r="745" spans="1:1">
-      <c r="A745" s="2"/>
-    </row>
-    <row r="746" spans="1:1">
-      <c r="A746" s="2"/>
-    </row>
-    <row r="747" spans="1:1">
-      <c r="A747" s="2"/>
-    </row>
-    <row r="748" spans="1:1">
-      <c r="A748" s="2"/>
-    </row>
-    <row r="749" spans="1:1">
-      <c r="A749" s="2"/>
-    </row>
-    <row r="750" spans="1:1">
-      <c r="A750" s="2"/>
-    </row>
-    <row r="751" spans="1:1">
-      <c r="A751" s="2"/>
-    </row>
-    <row r="752" spans="1:1">
-      <c r="A752" s="2"/>
-    </row>
-    <row r="753" spans="1:1">
-      <c r="A753" s="2"/>
-    </row>
-    <row r="754" spans="1:1">
-      <c r="A754" s="2"/>
-    </row>
-    <row r="755" spans="1:1">
-      <c r="A755" s="2"/>
-    </row>
-    <row r="756" spans="1:1">
-      <c r="A756" s="2"/>
-    </row>
-    <row r="757" spans="1:1">
-      <c r="A757" s="2"/>
-    </row>
-    <row r="758" spans="1:1">
-      <c r="A758" s="2"/>
-    </row>
-    <row r="759" spans="1:1">
-      <c r="A759" s="2"/>
-    </row>
-    <row r="760" spans="1:1">
-      <c r="A760" s="2"/>
-    </row>
-    <row r="761" spans="1:1">
-      <c r="A761" s="2"/>
-    </row>
-    <row r="762" spans="1:1">
-      <c r="A762" s="2"/>
-    </row>
-    <row r="763" spans="1:1">
-      <c r="A763" s="2"/>
-    </row>
-    <row r="764" spans="1:1">
-      <c r="A764" s="2"/>
-    </row>
-    <row r="765" spans="1:1">
-      <c r="A765" s="2"/>
-    </row>
-    <row r="766" spans="1:1">
-      <c r="A766" s="2"/>
-    </row>
-    <row r="767" spans="1:1">
-      <c r="A767" s="2"/>
-    </row>
-    <row r="768" spans="1:1">
-      <c r="A768" s="2"/>
-    </row>
-    <row r="769" spans="1:1">
-      <c r="A769" s="2"/>
-    </row>
-    <row r="770" spans="1:1">
-      <c r="A770" s="2"/>
-    </row>
-    <row r="771" spans="1:1">
-      <c r="A771" s="2"/>
-    </row>
-    <row r="772" spans="1:1">
-      <c r="A772" s="2"/>
-    </row>
-    <row r="773" spans="1:1">
-      <c r="A773" s="2"/>
-    </row>
-    <row r="774" spans="1:1">
-      <c r="A774" s="2"/>
-    </row>
-    <row r="775" spans="1:1">
-      <c r="A775" s="2"/>
-    </row>
-    <row r="776" spans="1:1">
-      <c r="A776" s="2"/>
-    </row>
-    <row r="777" spans="1:1">
-      <c r="A777" s="2"/>
-    </row>
-    <row r="778" spans="1:1">
-      <c r="A778" s="2"/>
-    </row>
-    <row r="779" spans="1:1">
-      <c r="A779" s="2"/>
-    </row>
-    <row r="780" spans="1:1">
-      <c r="A780" s="2"/>
-    </row>
-    <row r="781" spans="1:1">
-      <c r="A781" s="2"/>
-    </row>
-    <row r="782" spans="1:1">
-      <c r="A782" s="2"/>
-    </row>
-    <row r="783" spans="1:1">
-      <c r="A783" s="2"/>
-    </row>
-    <row r="784" spans="1:1">
-      <c r="A784" s="2"/>
-    </row>
-    <row r="785" spans="1:1">
-      <c r="A785" s="2"/>
-    </row>
-    <row r="786" spans="1:1">
-      <c r="A786" s="2"/>
-    </row>
-    <row r="787" spans="1:1">
-      <c r="A787" s="2"/>
-    </row>
-    <row r="788" spans="1:1">
-      <c r="A788" s="2"/>
-    </row>
-    <row r="789" spans="1:1">
-      <c r="A789" s="2"/>
-    </row>
-    <row r="790" spans="1:1">
-      <c r="A790" s="2"/>
-    </row>
-    <row r="791" spans="1:1">
-      <c r="A791" s="2"/>
-    </row>
-    <row r="792" spans="1:1">
-      <c r="A792" s="2"/>
-    </row>
-    <row r="793" spans="1:1">
-      <c r="A793" s="2"/>
-    </row>
-    <row r="794" spans="1:1">
-      <c r="A794" s="2"/>
-    </row>
-    <row r="795" spans="1:1">
-      <c r="A795" s="2"/>
-    </row>
-    <row r="796" spans="1:1">
-      <c r="A796" s="2"/>
-    </row>
-    <row r="797" spans="1:1">
-      <c r="A797" s="2"/>
-    </row>
-    <row r="798" spans="1:1">
-      <c r="A798" s="2"/>
-    </row>
-    <row r="799" spans="1:1">
-      <c r="A799" s="2"/>
-    </row>
-    <row r="800" spans="1:1">
-      <c r="A800" s="2"/>
-    </row>
-    <row r="801" spans="1:1">
-      <c r="A801" s="2"/>
-    </row>
-    <row r="802" spans="1:1">
-      <c r="A802" s="2"/>
-    </row>
-    <row r="803" spans="1:1">
-      <c r="A803" s="2"/>
-    </row>
-    <row r="804" spans="1:1">
-      <c r="A804" s="2"/>
-    </row>
-    <row r="805" spans="1:1">
-      <c r="A805" s="2"/>
-    </row>
-    <row r="806" spans="1:1">
-      <c r="A806" s="2"/>
-    </row>
-    <row r="807" spans="1:1">
-      <c r="A807" s="2"/>
-    </row>
-    <row r="808" spans="1:1">
-      <c r="A808" s="2"/>
-    </row>
-    <row r="809" spans="1:1">
-      <c r="A809" s="2"/>
-    </row>
-    <row r="810" spans="1:1">
-      <c r="A810" s="2"/>
-    </row>
-    <row r="811" spans="1:1">
-      <c r="A811" s="2"/>
-    </row>
-    <row r="812" spans="1:1">
-      <c r="A812" s="2"/>
-    </row>
-    <row r="813" spans="1:1">
-      <c r="A813" s="2"/>
-    </row>
-    <row r="814" spans="1:1">
-      <c r="A814" s="2"/>
-    </row>
-    <row r="815" spans="1:1">
-      <c r="A815" s="2"/>
-    </row>
-    <row r="816" spans="1:1">
-      <c r="A816" s="2"/>
-    </row>
-    <row r="817" spans="1:1">
-      <c r="A817" s="2"/>
-    </row>
-    <row r="818" spans="1:1">
-      <c r="A818" s="2"/>
-    </row>
-    <row r="819" spans="1:1">
-      <c r="A819" s="2"/>
-    </row>
-    <row r="820" spans="1:1">
-      <c r="A820" s="2"/>
-    </row>
-    <row r="821" spans="1:1">
-      <c r="A821" s="2"/>
-    </row>
-    <row r="822" spans="1:1">
-      <c r="A822" s="2"/>
-    </row>
-    <row r="823" spans="1:1">
-      <c r="A823" s="2"/>
-    </row>
-    <row r="824" spans="1:1">
-      <c r="A824" s="2"/>
-    </row>
-    <row r="825" spans="1:1">
-      <c r="A825" s="2"/>
-    </row>
-    <row r="826" spans="1:1">
-      <c r="A826" s="2"/>
-    </row>
-    <row r="827" spans="1:1">
-      <c r="A827" s="2"/>
-    </row>
-    <row r="828" spans="1:1">
-      <c r="A828" s="2"/>
-    </row>
-    <row r="829" spans="1:1">
-      <c r="A829" s="2"/>
-    </row>
-    <row r="830" spans="1:1">
-      <c r="A830" s="2"/>
-    </row>
-    <row r="831" spans="1:1">
-      <c r="A831" s="2"/>
-    </row>
-    <row r="832" spans="1:1">
-      <c r="A832" s="2"/>
-    </row>
-    <row r="833" spans="1:1">
-      <c r="A833" s="2"/>
-    </row>
-    <row r="834" spans="1:1">
-      <c r="A834" s="2"/>
-    </row>
-    <row r="835" spans="1:1">
-      <c r="A835" s="2"/>
-    </row>
-    <row r="836" spans="1:1">
-      <c r="A836" s="2"/>
-    </row>
-    <row r="837" spans="1:1">
-      <c r="A837" s="2"/>
-    </row>
-    <row r="838" spans="1:1">
-      <c r="A838" s="2"/>
-    </row>
-    <row r="839" spans="1:1">
-      <c r="A839" s="2"/>
-    </row>
-    <row r="840" spans="1:1">
-      <c r="A840" s="2"/>
-    </row>
-    <row r="841" spans="1:1">
-      <c r="A841" s="2"/>
-    </row>
-    <row r="842" spans="1:1">
-      <c r="A842" s="2"/>
-    </row>
-    <row r="843" spans="1:1">
-      <c r="A843" s="2"/>
-    </row>
-    <row r="844" spans="1:1">
-      <c r="A844" s="2"/>
-    </row>
-    <row r="845" spans="1:1">
-      <c r="A845" s="2"/>
-    </row>
-    <row r="846" spans="1:1">
-      <c r="A846" s="2"/>
-    </row>
-    <row r="847" spans="1:1">
-      <c r="A847" s="2"/>
-    </row>
-    <row r="848" spans="1:1">
-      <c r="A848" s="2"/>
-    </row>
-    <row r="849" spans="1:1">
-      <c r="A849" s="2"/>
-    </row>
-    <row r="850" spans="1:1">
-      <c r="A850" s="2"/>
-    </row>
-    <row r="851" spans="1:1">
-      <c r="A851" s="2"/>
-    </row>
-    <row r="852" spans="1:1">
-      <c r="A852" s="2"/>
-    </row>
-    <row r="853" spans="1:1">
-      <c r="A853" s="2"/>
-    </row>
-    <row r="854" spans="1:1">
-      <c r="A854" s="2"/>
-    </row>
-    <row r="855" spans="1:1">
-      <c r="A855" s="2"/>
-    </row>
-    <row r="856" spans="1:1">
-      <c r="A856" s="2"/>
-    </row>
-    <row r="857" spans="1:1">
-      <c r="A857" s="2"/>
-    </row>
-    <row r="858" spans="1:1">
-      <c r="A858" s="2"/>
-    </row>
-    <row r="859" spans="1:1">
-      <c r="A859" s="2"/>
-    </row>
-    <row r="860" spans="1:1">
-      <c r="A860" s="2"/>
-    </row>
-    <row r="861" spans="1:1">
-      <c r="A861" s="2"/>
-    </row>
-    <row r="862" spans="1:1">
-      <c r="A862" s="2"/>
-    </row>
-    <row r="863" spans="1:1">
-      <c r="A863" s="2"/>
-    </row>
-    <row r="864" spans="1:1">
-      <c r="A864" s="2"/>
-    </row>
-    <row r="865" spans="1:1">
-      <c r="A865" s="2"/>
-    </row>
-    <row r="866" spans="1:1">
-      <c r="A866" s="2"/>
-    </row>
-    <row r="867" spans="1:1">
-      <c r="A867" s="2"/>
-    </row>
-    <row r="868" spans="1:1">
-      <c r="A868" s="2"/>
-    </row>
-    <row r="869" spans="1:1">
-      <c r="A869" s="2"/>
-    </row>
-    <row r="870" spans="1:1">
-      <c r="A870" s="2"/>
-    </row>
-    <row r="871" spans="1:1">
-      <c r="A871" s="2"/>
-    </row>
-    <row r="872" spans="1:1">
-      <c r="A872" s="2"/>
-    </row>
-    <row r="873" spans="1:1">
-      <c r="A873" s="2"/>
-    </row>
-    <row r="874" spans="1:1">
-      <c r="A874" s="2"/>
-    </row>
-    <row r="875" spans="1:1">
-      <c r="A875" s="2"/>
-    </row>
-    <row r="876" spans="1:1">
-      <c r="A876" s="2"/>
-    </row>
-    <row r="877" spans="1:1">
-      <c r="A877" s="2"/>
-    </row>
-    <row r="878" spans="1:1">
-      <c r="A878" s="2"/>
-    </row>
-    <row r="879" spans="1:1">
-      <c r="A879" s="2"/>
-    </row>
-    <row r="880" spans="1:1">
-      <c r="A880" s="2"/>
-    </row>
-    <row r="881" spans="1:1">
-      <c r="A881" s="2"/>
-    </row>
-    <row r="882" spans="1:1">
-      <c r="A882" s="2"/>
-    </row>
-    <row r="883" spans="1:1">
-      <c r="A883" s="2"/>
-    </row>
-    <row r="884" spans="1:1">
-      <c r="A884" s="2"/>
-    </row>
-    <row r="885" spans="1:1">
-      <c r="A885" s="2"/>
-    </row>
-    <row r="886" spans="1:1">
-      <c r="A886" s="2"/>
-    </row>
-    <row r="887" spans="1:1">
-      <c r="A887" s="2"/>
-    </row>
-    <row r="888" spans="1:1">
-      <c r="A888" s="2"/>
-    </row>
-    <row r="889" spans="1:1">
-      <c r="A889" s="2"/>
-    </row>
-    <row r="890" spans="1:1">
-      <c r="A890" s="2"/>
-    </row>
-    <row r="891" spans="1:1">
-      <c r="A891" s="2"/>
-    </row>
-    <row r="892" spans="1:1">
-      <c r="A892" s="2"/>
-    </row>
-    <row r="893" spans="1:1">
-      <c r="A893" s="2"/>
-    </row>
-    <row r="894" spans="1:1">
-      <c r="A894" s="2"/>
-    </row>
-    <row r="895" spans="1:1">
-      <c r="A895" s="2"/>
-    </row>
-    <row r="896" spans="1:1">
-      <c r="A896" s="2"/>
-    </row>
-    <row r="897" spans="1:1">
-      <c r="A897" s="2"/>
-    </row>
-    <row r="898" spans="1:1">
-      <c r="A898" s="2"/>
-    </row>
-    <row r="899" spans="1:1">
-      <c r="A899" s="2"/>
-    </row>
-    <row r="900" spans="1:1">
-      <c r="A900" s="2"/>
-    </row>
-    <row r="901" spans="1:1">
-      <c r="A901" s="2"/>
-    </row>
-    <row r="902" spans="1:1">
-      <c r="A902" s="2"/>
-    </row>
-    <row r="903" spans="1:1">
-      <c r="A903" s="2"/>
-    </row>
-    <row r="904" spans="1:1">
-      <c r="A904" s="2"/>
-    </row>
-    <row r="905" spans="1:1">
-      <c r="A905" s="2"/>
-    </row>
-    <row r="906" spans="1:1">
-      <c r="A906" s="2"/>
-    </row>
-    <row r="907" spans="1:1">
-      <c r="A907" s="2"/>
-    </row>
-    <row r="908" spans="1:1">
-      <c r="A908" s="2"/>
-    </row>
-    <row r="909" spans="1:1">
-      <c r="A909" s="2"/>
-    </row>
-    <row r="910" spans="1:1">
-      <c r="A910" s="2"/>
-    </row>
-    <row r="911" spans="1:1">
-      <c r="A911" s="2"/>
-    </row>
-    <row r="912" spans="1:1">
-      <c r="A912" s="2"/>
-    </row>
-    <row r="913" spans="1:1">
-      <c r="A913" s="2"/>
-    </row>
-    <row r="914" spans="1:1">
-      <c r="A914" s="2"/>
-    </row>
-    <row r="915" spans="1:1">
-      <c r="A915" s="2"/>
-    </row>
-    <row r="916" spans="1:1">
-      <c r="A916" s="2"/>
-    </row>
-    <row r="917" spans="1:1">
-      <c r="A917" s="2"/>
-    </row>
-    <row r="918" spans="1:1">
-      <c r="A918" s="2"/>
-    </row>
-    <row r="919" spans="1:1">
-      <c r="A919" s="2"/>
-    </row>
-    <row r="920" spans="1:1">
-      <c r="A920" s="2"/>
-    </row>
-    <row r="921" spans="1:1">
-      <c r="A921" s="2"/>
-    </row>
-    <row r="922" spans="1:1">
-      <c r="A922" s="2"/>
-    </row>
-    <row r="923" spans="1:1">
-      <c r="A923" s="2"/>
-    </row>
-    <row r="924" spans="1:1">
-      <c r="A924" s="2"/>
-    </row>
-    <row r="925" spans="1:1">
-      <c r="A925" s="2"/>
-    </row>
-    <row r="926" spans="1:1">
-      <c r="A926" s="2"/>
-    </row>
-    <row r="927" spans="1:1">
-      <c r="A927" s="2"/>
-    </row>
-    <row r="928" spans="1:1">
-      <c r="A928" s="2"/>
-    </row>
-    <row r="929" spans="1:1">
-      <c r="A929" s="2"/>
-    </row>
-    <row r="930" spans="1:1">
-      <c r="A930" s="2"/>
-    </row>
-    <row r="931" spans="1:1">
-      <c r="A931" s="2"/>
-    </row>
-    <row r="932" spans="1:1">
-      <c r="A932" s="2"/>
-    </row>
-    <row r="933" spans="1:1">
-      <c r="A933" s="2"/>
-    </row>
-    <row r="934" spans="1:1">
-      <c r="A934" s="2"/>
-    </row>
-    <row r="935" spans="1:1">
-      <c r="A935" s="2"/>
-    </row>
-    <row r="936" spans="1:1">
-      <c r="A936" s="2"/>
-    </row>
-    <row r="937" spans="1:1">
-      <c r="A937" s="2"/>
-    </row>
-    <row r="938" spans="1:1">
-      <c r="A938" s="2"/>
-    </row>
-    <row r="939" spans="1:1">
-      <c r="A939" s="2"/>
-    </row>
-    <row r="940" spans="1:1">
-      <c r="A940" s="2"/>
-    </row>
-    <row r="941" spans="1:1">
-      <c r="A941" s="2"/>
-    </row>
-    <row r="942" spans="1:1">
-      <c r="A942" s="2"/>
-    </row>
-    <row r="943" spans="1:1">
-      <c r="A943" s="2"/>
-    </row>
-    <row r="944" spans="1:1">
-      <c r="A944" s="2"/>
-    </row>
-    <row r="945" spans="1:1">
-      <c r="A945" s="2"/>
-    </row>
-    <row r="946" spans="1:1">
-      <c r="A946" s="2"/>
-    </row>
-    <row r="947" spans="1:1">
-      <c r="A947" s="2"/>
-    </row>
-    <row r="948" spans="1:1">
-      <c r="A948" s="2"/>
-    </row>
-    <row r="949" spans="1:1">
-      <c r="A949" s="2"/>
-    </row>
-    <row r="950" spans="1:1">
-      <c r="A950" s="2"/>
-    </row>
-    <row r="951" spans="1:1">
-      <c r="A951" s="2"/>
-    </row>
-    <row r="952" spans="1:1">
-      <c r="A952" s="2"/>
-    </row>
-    <row r="953" spans="1:1">
-      <c r="A953" s="2"/>
-    </row>
-    <row r="954" spans="1:1">
-      <c r="A954" s="2"/>
-    </row>
-    <row r="955" spans="1:1">
-      <c r="A955" s="2"/>
-    </row>
-    <row r="956" spans="1:1">
-      <c r="A956" s="2"/>
-    </row>
-    <row r="957" spans="1:1">
-      <c r="A957" s="2"/>
-    </row>
-    <row r="958" spans="1:1">
-      <c r="A958" s="2"/>
-    </row>
-    <row r="959" spans="1:1">
-      <c r="A959" s="2"/>
-    </row>
-    <row r="960" spans="1:1">
-      <c r="A960" s="2"/>
-    </row>
-    <row r="961" spans="1:1">
-      <c r="A961" s="2"/>
-    </row>
-    <row r="962" spans="1:1">
-      <c r="A962" s="2"/>
-    </row>
-    <row r="963" spans="1:1">
-      <c r="A963" s="2"/>
-    </row>
-    <row r="964" spans="1:1">
-      <c r="A964" s="2"/>
-    </row>
-    <row r="965" spans="1:1">
-      <c r="A965" s="2"/>
-    </row>
-    <row r="966" spans="1:1">
-      <c r="A966" s="2"/>
-    </row>
-    <row r="967" spans="1:1">
-      <c r="A967" s="2"/>
-    </row>
-    <row r="968" spans="1:1">
-      <c r="A968" s="2"/>
-    </row>
-    <row r="969" spans="1:1">
-      <c r="A969" s="2"/>
-    </row>
-    <row r="970" spans="1:1">
-      <c r="A970" s="2"/>
-    </row>
-    <row r="971" spans="1:1">
-      <c r="A971" s="2"/>
-    </row>
-    <row r="972" spans="1:1">
-      <c r="A972" s="2"/>
-    </row>
-    <row r="973" spans="1:1">
-      <c r="A973" s="2"/>
-    </row>
-    <row r="974" spans="1:1">
-      <c r="A974" s="2"/>
-    </row>
-    <row r="975" spans="1:1">
-      <c r="A975" s="2"/>
-    </row>
-    <row r="976" spans="1:1">
-      <c r="A976" s="2"/>
-    </row>
-    <row r="977" spans="1:1">
-      <c r="A977" s="2"/>
-    </row>
-    <row r="978" spans="1:1">
-      <c r="A978" s="2"/>
-    </row>
-    <row r="979" spans="1:1">
-      <c r="A979" s="2"/>
-    </row>
-    <row r="980" spans="1:1">
-      <c r="A980" s="2"/>
-    </row>
-    <row r="981" spans="1:1">
-      <c r="A981" s="2"/>
-    </row>
-    <row r="982" spans="1:1">
-      <c r="A982" s="2"/>
-    </row>
-    <row r="983" spans="1:1">
-      <c r="A983" s="2"/>
-    </row>
-    <row r="984" spans="1:1">
-      <c r="A984" s="2"/>
-    </row>
-    <row r="985" spans="1:1">
-      <c r="A985" s="2"/>
-    </row>
-    <row r="986" spans="1:1">
-      <c r="A986" s="2"/>
-    </row>
-    <row r="987" spans="1:1">
-      <c r="A987" s="2"/>
-    </row>
-    <row r="988" spans="1:1">
-      <c r="A988" s="2"/>
-    </row>
-    <row r="989" spans="1:1">
-      <c r="A989" s="2"/>
-    </row>
-    <row r="990" spans="1:1">
-      <c r="A990" s="2"/>
-    </row>
-    <row r="991" spans="1:1">
-      <c r="A991" s="2"/>
-    </row>
-    <row r="992" spans="1:1">
-      <c r="A992" s="2"/>
-    </row>
-    <row r="993" spans="1:1">
-      <c r="A993" s="2"/>
-    </row>
-    <row r="994" spans="1:1">
-      <c r="A994" s="2"/>
-    </row>
-    <row r="995" spans="1:1">
-      <c r="A995" s="2"/>
-    </row>
-    <row r="996" spans="1:1">
-      <c r="A996" s="2"/>
-    </row>
-    <row r="997" spans="1:1">
-      <c r="A997" s="2"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:A18"/>

</xml_diff>

<commit_message>
Add contain example command with user-account target
</commit_message>
<xml_diff>
--- a/docs/targets.xlsx
+++ b/docs/targets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835"/>
+    <workbookView xWindow="390" yWindow="675" windowWidth="18855" windowHeight="8835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="128">
   <si>
     <t>Target Type</t>
   </si>
@@ -750,6 +750,41 @@
     version     STRING OPTIONAL
 }</t>
   </si>
+  <si>
+    <t>user-account ::= MAP {
+    user_id                 [1] STRING,
+    account_login           [2] STRING OPTIONAL,
+    account_type            [3] STRING OPTIONAL,
+    display_name            [4] STRING OPTIONAL,
+    is_service_account      [5] BOOLEAN OPTIONAL,
+    is_privileged           [6] BOOLEAN OPTIONAL,
+    can_escalate_privs      [7] BOOLEAN OPTIONAL,
+    is_disabled             [8] BOOLEAN OPTIONAL,
+    account_created         [9] DateTime OPTIONAL,
+    account_expires        [10] DateTime OPTIONAL,
+    password_last_changed  [11] DateTime OPTIONAL,
+    account_first_login    [12] DateTime OPTIONAL,
+    account_last_login     [13] DateTime OPTIONAL
+}
+account-type ::= ENUMERATED {
+    unix            (1),
+    windows-local   (2),
+    windows-domain  (3),
+    ldap            (4),
+    tacacs          (5),
+    radius          (6),
+    nis             (7),
+    openid          (8),
+    facebook        (9),
+    skype           (10),
+    twitter         (11)
+}</t>
+  </si>
+  <si>
+    <t>{ "action": "contain",
+  "target": {
+    "user-account": {</t>
+  </si>
 </sst>
 </file>
 
@@ -1250,9 +1285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -31479,8 +31514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -31700,12 +31735,16 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="326.25">
       <c r="A22" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:4">

</xml_diff>